<commit_message>
move unused files to old file location. Need to find a way to modify old code to compare results, to ensure that everything is working as well as it was before reorganization
</commit_message>
<xml_diff>
--- a/currently_in_use/Experimental_Results.xlsx
+++ b/currently_in_use/Experimental_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\git-repos\Overexposure\currently_in_use\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71C0DE4-7EBC-423C-B57D-C8D8CEEE1AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CB0FDC-CD18-48D5-924A-979CB0CC2EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="payoff" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">payoff!$A$1:$L$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">runtimes!$A$1:$L$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">runtimes!$A$1:$L$21</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="28">
   <si>
     <t>Num Nodes</t>
   </si>
@@ -163,7 +163,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -186,11 +186,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -201,11 +214,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFCC4C4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -499,11 +520,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD15"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,31 +874,31 @@
         <v>0.5</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" s="2">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G9" s="2">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="H9" s="2">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J9" s="2">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="K9" s="2">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="L9" s="2">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="U9" s="7"/>
     </row>
@@ -892,31 +913,31 @@
         <v>0.5</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E10" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F10" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G10" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H10" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J10" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K10" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L10" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="U10" s="7"/>
     </row>
@@ -934,200 +955,516 @@
         <v>18</v>
       </c>
       <c r="E11" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F11" s="2">
+        <v>6</v>
+      </c>
+      <c r="G11" s="2">
+        <v>3</v>
+      </c>
+      <c r="H11" s="2">
+        <v>3</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="2">
+        <v>4</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>4</v>
+      </c>
+      <c r="U11" s="7"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>100</v>
+      </c>
+      <c r="B12" s="2">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>6</v>
+      </c>
+      <c r="G12" s="2">
+        <v>3</v>
+      </c>
+      <c r="H12" s="2">
+        <v>3</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="2">
+        <v>4</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>4</v>
+      </c>
+      <c r="U12" s="7"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>100</v>
+      </c>
+      <c r="B13" s="2">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2</v>
+      </c>
+      <c r="F13" s="2">
+        <v>6</v>
+      </c>
+      <c r="G13" s="2">
+        <v>3</v>
+      </c>
+      <c r="H13" s="2">
+        <v>3</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="2">
+        <v>4</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>4</v>
+      </c>
+      <c r="U13" s="7"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>100</v>
+      </c>
+      <c r="B14" s="2">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>6</v>
+      </c>
+      <c r="G14" s="2">
+        <v>3</v>
+      </c>
+      <c r="H14" s="2">
+        <v>3</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="2">
+        <v>4</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <v>4</v>
+      </c>
+      <c r="U14" s="7"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>100</v>
+      </c>
+      <c r="B15" s="2">
+        <v>5</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2</v>
+      </c>
+      <c r="F15" s="2">
+        <v>6</v>
+      </c>
+      <c r="G15" s="2">
+        <v>3</v>
+      </c>
+      <c r="H15" s="2">
+        <v>3</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="2">
+        <v>4</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>4</v>
+      </c>
+      <c r="U15" s="7"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>100</v>
+      </c>
+      <c r="B16" s="2">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>6</v>
+      </c>
+      <c r="G16" s="2">
+        <v>3</v>
+      </c>
+      <c r="H16" s="2">
+        <v>3</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="2">
+        <v>4</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
+        <v>4</v>
+      </c>
+      <c r="U16" s="7"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>100</v>
+      </c>
+      <c r="B17" s="2">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="2">
+        <v>3</v>
+      </c>
+      <c r="F17" s="2">
+        <v>18</v>
+      </c>
+      <c r="G17" s="2">
+        <v>15</v>
+      </c>
+      <c r="H17" s="2">
+        <v>15</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="2">
+        <v>17</v>
+      </c>
+      <c r="K17" s="2">
+        <v>17</v>
+      </c>
+      <c r="L17" s="2">
+        <v>17</v>
+      </c>
+      <c r="U17" s="7"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>100</v>
+      </c>
+      <c r="B18" s="2">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="2">
+        <v>4</v>
+      </c>
+      <c r="F18" s="2">
+        <v>9</v>
+      </c>
+      <c r="G18" s="2">
+        <v>6</v>
+      </c>
+      <c r="H18" s="2">
+        <v>6</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="2">
+        <v>6</v>
+      </c>
+      <c r="K18" s="2">
+        <v>6</v>
+      </c>
+      <c r="L18" s="2">
+        <v>6</v>
+      </c>
+      <c r="U18" s="7"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>100</v>
+      </c>
+      <c r="B19" s="2">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2">
         <v>12</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G19" s="2">
         <v>13</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H19" s="2">
         <v>13</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="2">
+      <c r="I19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="2">
         <v>13</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K19" s="2">
         <v>13</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L19" s="2">
         <v>13</v>
       </c>
-      <c r="U11" s="7"/>
-    </row>
-    <row r="12" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>100</v>
-      </c>
-      <c r="B12" s="2">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="U19" s="7"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>100</v>
+      </c>
+      <c r="B20" s="2">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E20" s="2">
         <v>6</v>
       </c>
-      <c r="F12" s="2">
-        <v>5</v>
-      </c>
-      <c r="G12" s="2">
-        <v>2</v>
-      </c>
-      <c r="H12" s="2">
-        <v>4</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" s="2">
-        <v>5</v>
-      </c>
-      <c r="K12" s="2">
-        <v>3</v>
-      </c>
-      <c r="L12" s="2">
-        <v>5</v>
-      </c>
-      <c r="M12" s="7"/>
-      <c r="U12" s="7"/>
-    </row>
-    <row r="13" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>100</v>
-      </c>
-      <c r="B13" s="2">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="F20" s="2">
+        <v>5</v>
+      </c>
+      <c r="G20" s="2">
+        <v>2</v>
+      </c>
+      <c r="H20" s="2">
+        <v>4</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="2">
+        <v>5</v>
+      </c>
+      <c r="K20" s="2">
+        <v>3</v>
+      </c>
+      <c r="L20" s="2">
+        <v>5</v>
+      </c>
+      <c r="U20" s="7"/>
+    </row>
+    <row r="21" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>100</v>
+      </c>
+      <c r="B21" s="2">
+        <v>5</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E21" s="2">
         <v>7</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F21" s="2">
         <v>1</v>
       </c>
-      <c r="G13" s="2">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="2">
+      <c r="G21" s="2">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="2">
         <v>8</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K21" s="2">
         <v>8</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L21" s="2">
         <v>8</v>
       </c>
-      <c r="M13" s="7"/>
-      <c r="U13" s="7"/>
-    </row>
-    <row r="14" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>100</v>
-      </c>
-      <c r="B14" s="2">
-        <v>5</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="2">
+      <c r="M21" s="7"/>
+      <c r="U21" s="7"/>
+    </row>
+    <row r="22" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>100</v>
+      </c>
+      <c r="B22" s="2">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="2">
         <v>8</v>
       </c>
-      <c r="F14" s="2">
-        <v>5</v>
-      </c>
-      <c r="G14" s="2">
-        <v>3</v>
-      </c>
-      <c r="H14" s="2">
-        <v>3</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="2">
-        <v>4</v>
-      </c>
-      <c r="K14" s="2">
-        <v>2</v>
-      </c>
-      <c r="L14" s="2">
-        <v>4</v>
-      </c>
-      <c r="M14" s="7"/>
-      <c r="U14" s="7"/>
-    </row>
-    <row r="15" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>100</v>
-      </c>
-      <c r="B15" s="2">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="F22" s="2">
+        <v>5</v>
+      </c>
+      <c r="G22" s="2">
+        <v>3</v>
+      </c>
+      <c r="H22" s="2">
+        <v>3</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="2">
+        <v>4</v>
+      </c>
+      <c r="K22" s="2">
+        <v>2</v>
+      </c>
+      <c r="L22" s="2">
+        <v>4</v>
+      </c>
+      <c r="M22" s="7"/>
+      <c r="U22" s="7"/>
+    </row>
+    <row r="23" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>100</v>
+      </c>
+      <c r="B23" s="2">
+        <v>5</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E23" s="2">
         <v>9</v>
       </c>
-      <c r="F15" s="2">
-        <v>2</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2">
+      <c r="F23" s="2">
+        <v>2</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
         <v>1</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="2">
+      <c r="I23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="2">
         <v>1</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K23" s="2">
         <v>1</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L23" s="2">
         <v>1</v>
       </c>
-      <c r="M15" s="7"/>
-      <c r="U15" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="U23" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L2" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L15">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L23">
       <sortCondition ref="E1:E2"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="F2:K15">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="F2:K20">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>AND(F2&gt;$L2, NOT(F2 = "-"))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21:K23">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(F21&gt;$L21, NOT(F21 = "-"))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1137,11 +1474,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U16"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1540,31 +1877,31 @@
         <v>0.5</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" s="2">
-        <v>7.510000000001682E-4</v>
+        <v>3.4840000000002652E-4</v>
       </c>
       <c r="G9" s="2">
-        <v>4.010000000009839E-5</v>
+        <v>3.5000000000007248E-5</v>
       </c>
       <c r="H9" s="2">
-        <v>2.0335999999998582E-3</v>
+        <v>5.7809999999991479E-4</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J9" s="2">
-        <v>2.9578499999999949E-2</v>
+        <v>3.7653399999999948E-2</v>
       </c>
       <c r="K9" s="2">
-        <v>1.4114999999996769E-3</v>
+        <v>9.9870000000001902E-4</v>
       </c>
       <c r="L9" s="2">
-        <v>3.7574999999998582E-3</v>
+        <v>3.4846999999998962E-3</v>
       </c>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
@@ -1586,31 +1923,31 @@
         <v>0.5</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E10" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F10" s="2">
-        <v>8.7480000000006441E-4</v>
+        <v>3.2960000000004103E-4</v>
       </c>
       <c r="G10" s="2">
-        <v>4.5900000000043129E-5</v>
+        <v>3.3799999999972741E-5</v>
       </c>
       <c r="H10" s="2">
-        <v>1.9746999999999959E-3</v>
+        <v>7.6709999999990952E-4</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J10" s="2">
-        <v>0.12664510000000009</v>
+        <v>3.3009400000000078E-2</v>
       </c>
       <c r="K10" s="2">
-        <v>1.015699999999953E-3</v>
+        <v>1.105500000000093E-3</v>
       </c>
       <c r="L10" s="2">
-        <v>3.6270000000000469E-3</v>
+        <v>3.3337999999999419E-3</v>
       </c>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
@@ -1635,28 +1972,28 @@
         <v>18</v>
       </c>
       <c r="E11" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F11" s="2">
-        <v>8.8819999999989463E-4</v>
+        <v>5.0209999999994981E-4</v>
       </c>
       <c r="G11" s="2">
-        <v>4.0000000000262048E-5</v>
+        <v>5.2099999999999369E-5</v>
       </c>
       <c r="H11" s="2">
-        <v>3.5446000000001199E-3</v>
+        <v>5.4239999999994293E-4</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J11" s="2">
-        <v>2.7614599999999712E-2</v>
+        <v>3.5348899999999912E-2</v>
       </c>
       <c r="K11" s="2">
-        <v>9.5620000000007366E-4</v>
+        <v>2.2324000000000228E-3</v>
       </c>
       <c r="L11" s="2">
-        <v>3.4659999999999691E-3</v>
+        <v>3.3706999999999492E-3</v>
       </c>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
@@ -1667,7 +2004,7 @@
       <c r="T11" s="8"/>
       <c r="U11" s="7"/>
     </row>
-    <row r="12" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>100</v>
       </c>
@@ -1678,31 +2015,31 @@
         <v>0.5</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F12" s="2">
-        <v>9.6989999999985699E-4</v>
+        <v>3.9710000000003909E-4</v>
       </c>
       <c r="G12" s="2">
-        <v>4.3999999999932982E-5</v>
+        <v>5.7799999999996743E-5</v>
       </c>
       <c r="H12" s="2">
-        <v>2.136600000000044E-3</v>
+        <v>5.8010000000008333E-4</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J12" s="2">
-        <v>3.1462200000000003E-2</v>
+        <v>3.608279999999997E-2</v>
       </c>
       <c r="K12" s="2">
-        <v>1.658700000000124E-3</v>
+        <v>1.2410000000000481E-3</v>
       </c>
       <c r="L12" s="2">
-        <v>3.7641999999999949E-3</v>
+        <v>3.6372000000000071E-3</v>
       </c>
       <c r="N12" s="8"/>
       <c r="O12" s="8"/>
@@ -1713,7 +2050,7 @@
       <c r="T12" s="8"/>
       <c r="U12" s="7"/>
     </row>
-    <row r="13" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>100</v>
       </c>
@@ -1724,31 +2061,31 @@
         <v>0.5</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E13" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F13" s="2">
-        <v>9.1099999999999515E-4</v>
+        <v>3.4259999999997071E-4</v>
       </c>
       <c r="G13" s="2">
-        <v>4.3300000000079393E-5</v>
+        <v>3.3400000000072261E-5</v>
       </c>
       <c r="H13" s="2">
-        <v>3.38879999999997E-3</v>
+        <v>5.6570000000000231E-4</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J13" s="2">
-        <v>3.3653700000000009E-2</v>
+        <v>3.3288299999999937E-2</v>
       </c>
       <c r="K13" s="2">
-        <v>9.9339999999992212E-4</v>
+        <v>1.2907999999999249E-3</v>
       </c>
       <c r="L13" s="2">
-        <v>3.3805999999999559E-3</v>
+        <v>3.3530999999999982E-3</v>
       </c>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
@@ -1759,7 +2096,7 @@
       <c r="T13" s="8"/>
       <c r="U13" s="7"/>
     </row>
-    <row r="14" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>100</v>
       </c>
@@ -1773,28 +2110,28 @@
         <v>18</v>
       </c>
       <c r="E14" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F14" s="2">
-        <v>9.820000000000384E-4</v>
+        <v>7.4200000000002042E-4</v>
       </c>
       <c r="G14" s="2">
-        <v>3.7700000000029377E-5</v>
+        <v>6.4099999999900348E-5</v>
       </c>
       <c r="H14" s="2">
-        <v>2.098300000000108E-3</v>
+        <v>8.1209999999987126E-4</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J14" s="2">
-        <v>3.0919099999999981E-2</v>
+        <v>3.5400199999999993E-2</v>
       </c>
       <c r="K14" s="2">
-        <v>1.442499999999791E-3</v>
+        <v>1.1413999999998481E-3</v>
       </c>
       <c r="L14" s="2">
-        <v>3.7827999999999751E-3</v>
+        <v>3.6249999999999889E-3</v>
       </c>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
@@ -1805,42 +2142,42 @@
       <c r="T14" s="8"/>
       <c r="U14" s="7"/>
     </row>
-    <row r="15" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>100</v>
-      </c>
-      <c r="B15" s="2">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="2">
-        <v>9</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1.345400000000385E-3</v>
-      </c>
-      <c r="G15" s="2">
-        <v>7.9899999999799576E-5</v>
-      </c>
-      <c r="H15" s="2">
-        <v>1.519300000000001E-3</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="2">
-        <v>2.8174400000000151E-2</v>
-      </c>
-      <c r="K15" s="2">
-        <v>1.4856000000000871E-3</v>
-      </c>
-      <c r="L15" s="2">
-        <v>3.2011999999999041E-3</v>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>100</v>
+      </c>
+      <c r="B15" s="10">
+        <v>5</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="10">
+        <v>2</v>
+      </c>
+      <c r="F15" s="10">
+        <v>3.3450000000001529E-4</v>
+      </c>
+      <c r="G15" s="10">
+        <v>3.4800000000001503E-5</v>
+      </c>
+      <c r="H15" s="10">
+        <v>5.5909999999992355E-4</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="10">
+        <v>3.5004999999999953E-2</v>
+      </c>
+      <c r="K15" s="10">
+        <v>1.2246000000000199E-3</v>
+      </c>
+      <c r="L15" s="10">
+        <v>4.0310999999999542E-3</v>
       </c>
       <c r="N15" s="8"/>
       <c r="O15" s="8"/>
@@ -1851,41 +2188,335 @@
       <c r="T15" s="8"/>
       <c r="U15" s="7"/>
     </row>
-    <row r="16" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="7"/>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>100</v>
+      </c>
+      <c r="B16" s="2">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>3.3620000000000871E-4</v>
+      </c>
+      <c r="G16" s="2">
+        <v>8.6299999999983612E-5</v>
+      </c>
+      <c r="H16" s="2">
+        <v>7.4099999999999167E-4</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="2">
+        <v>3.3232200000000052E-2</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1.3037000000000189E-3</v>
+      </c>
+      <c r="L16" s="2">
+        <v>3.0709999999999349E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>100</v>
+      </c>
+      <c r="B17" s="2">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="2">
+        <v>3</v>
+      </c>
+      <c r="F17" s="2">
+        <v>7.510000000001682E-4</v>
+      </c>
+      <c r="G17" s="2">
+        <v>4.010000000009839E-5</v>
+      </c>
+      <c r="H17" s="2">
+        <v>2.0335999999998582E-3</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="2">
+        <v>2.9578499999999949E-2</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1.4114999999996769E-3</v>
+      </c>
+      <c r="L17" s="2">
+        <v>3.7574999999998582E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>100</v>
+      </c>
+      <c r="B18" s="2">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="2">
+        <v>4</v>
+      </c>
+      <c r="F18" s="2">
+        <v>8.7480000000006441E-4</v>
+      </c>
+      <c r="G18" s="2">
+        <v>4.5900000000043129E-5</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1.9746999999999959E-3</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.12664510000000009</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1.015699999999953E-3</v>
+      </c>
+      <c r="L18" s="2">
+        <v>3.6270000000000469E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>100</v>
+      </c>
+      <c r="B19" s="2">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2">
+        <v>8.8819999999989463E-4</v>
+      </c>
+      <c r="G19" s="2">
+        <v>4.0000000000262048E-5</v>
+      </c>
+      <c r="H19" s="2">
+        <v>3.5446000000001199E-3</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="2">
+        <v>2.7614599999999712E-2</v>
+      </c>
+      <c r="K19" s="2">
+        <v>9.5620000000007366E-4</v>
+      </c>
+      <c r="L19" s="2">
+        <v>3.4659999999999691E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>100</v>
+      </c>
+      <c r="B20" s="2">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="2">
+        <v>6</v>
+      </c>
+      <c r="F20" s="2">
+        <v>9.6989999999985699E-4</v>
+      </c>
+      <c r="G20" s="2">
+        <v>4.3999999999932982E-5</v>
+      </c>
+      <c r="H20" s="2">
+        <v>2.136600000000044E-3</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="2">
+        <v>3.1462200000000003E-2</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1.658700000000124E-3</v>
+      </c>
+      <c r="L20" s="2">
+        <v>3.7641999999999949E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>100</v>
+      </c>
+      <c r="B21" s="2">
+        <v>5</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="2">
+        <v>7</v>
+      </c>
+      <c r="F21" s="2">
+        <v>9.1099999999999515E-4</v>
+      </c>
+      <c r="G21" s="2">
+        <v>4.3300000000079393E-5</v>
+      </c>
+      <c r="H21" s="2">
+        <v>3.38879999999997E-3</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="2">
+        <v>3.3653700000000009E-2</v>
+      </c>
+      <c r="K21" s="2">
+        <v>9.9339999999992212E-4</v>
+      </c>
+      <c r="L21" s="2">
+        <v>3.3805999999999559E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>100</v>
+      </c>
+      <c r="B22" s="2">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="2">
+        <v>8</v>
+      </c>
+      <c r="F22" s="2">
+        <v>9.820000000000384E-4</v>
+      </c>
+      <c r="G22" s="2">
+        <v>3.7700000000029377E-5</v>
+      </c>
+      <c r="H22" s="2">
+        <v>2.098300000000108E-3</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="2">
+        <v>3.0919099999999981E-2</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1.442499999999791E-3</v>
+      </c>
+      <c r="L22" s="2">
+        <v>3.7827999999999751E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>100</v>
+      </c>
+      <c r="B23" s="2">
+        <v>5</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="2">
+        <v>9</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1.345400000000385E-3</v>
+      </c>
+      <c r="G23" s="2">
+        <v>7.9899999999799576E-5</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1.519300000000001E-3</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="2">
+        <v>2.8174400000000151E-2</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1.4856000000000871E-3</v>
+      </c>
+      <c r="L23" s="2">
+        <v>3.2011999999999041E-3</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L2" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L15">
-      <sortCondition ref="E1:E2"/>
+  <autoFilter ref="A1:L21" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L23">
+      <sortCondition ref="E1:E21"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="L1">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:L16">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="F2:L20">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21:L23">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
remove weights for rejects in bipartite graph and make sure reject nodes are not in x_keys for bipartite ilp
</commit_message>
<xml_diff>
--- a/currently_in_use/Experimental_Results.xlsx
+++ b/currently_in_use/Experimental_Results.xlsx
@@ -502,7 +502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AY324"/>
+  <dimension ref="A1:AY328"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A314" ySplit="1"/>
@@ -38006,6 +38006,474 @@
         </is>
       </c>
       <c r="AA324" t="inlineStr">
+        <is>
+          <t>y_r_99</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>150</v>
+      </c>
+      <c r="B325" t="n">
+        <v>5</v>
+      </c>
+      <c r="C325" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>ER</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>test_files/SA1/ER/150/2.txt</t>
+        </is>
+      </c>
+      <c r="F325" t="n">
+        <v>8</v>
+      </c>
+      <c r="G325" t="n">
+        <v>10</v>
+      </c>
+      <c r="H325" t="n">
+        <v>10</v>
+      </c>
+      <c r="I325" t="n">
+        <v>10</v>
+      </c>
+      <c r="J325" t="n">
+        <v>10</v>
+      </c>
+      <c r="K325" t="n">
+        <v>10</v>
+      </c>
+      <c r="L325" t="n">
+        <v>10</v>
+      </c>
+      <c r="M325" t="inlineStr">
+        <is>
+          <t>x_0</t>
+        </is>
+      </c>
+      <c r="N325" t="inlineStr">
+        <is>
+          <t>x_1</t>
+        </is>
+      </c>
+      <c r="O325" t="inlineStr">
+        <is>
+          <t>x_2</t>
+        </is>
+      </c>
+      <c r="P325" t="inlineStr">
+        <is>
+          <t>x_4</t>
+        </is>
+      </c>
+      <c r="Q325" t="inlineStr">
+        <is>
+          <t>x_6</t>
+        </is>
+      </c>
+      <c r="R325" t="inlineStr">
+        <is>
+          <t>y_r_142</t>
+        </is>
+      </c>
+      <c r="S325" t="inlineStr">
+        <is>
+          <t>y_r_145</t>
+        </is>
+      </c>
+      <c r="T325" t="inlineStr">
+        <is>
+          <t>y_r_147</t>
+        </is>
+      </c>
+      <c r="U325" t="inlineStr">
+        <is>
+          <t>y_r_24</t>
+        </is>
+      </c>
+      <c r="V325" t="inlineStr">
+        <is>
+          <t>y_r_27</t>
+        </is>
+      </c>
+      <c r="W325" t="inlineStr">
+        <is>
+          <t>y_r_31</t>
+        </is>
+      </c>
+      <c r="X325" t="inlineStr">
+        <is>
+          <t>y_r_35</t>
+        </is>
+      </c>
+      <c r="Y325" t="inlineStr">
+        <is>
+          <t>y_r_74</t>
+        </is>
+      </c>
+      <c r="Z325" t="inlineStr">
+        <is>
+          <t>y_r_85</t>
+        </is>
+      </c>
+      <c r="AA325" t="inlineStr">
+        <is>
+          <t>y_r_99</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>150</v>
+      </c>
+      <c r="B326" t="n">
+        <v>5</v>
+      </c>
+      <c r="C326" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>ER</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>test_files/SA1/ER/150/2.txt</t>
+        </is>
+      </c>
+      <c r="F326" t="n">
+        <v>8</v>
+      </c>
+      <c r="G326" t="n">
+        <v>10</v>
+      </c>
+      <c r="H326" t="n">
+        <v>10</v>
+      </c>
+      <c r="I326" t="n">
+        <v>10</v>
+      </c>
+      <c r="J326" t="n">
+        <v>10</v>
+      </c>
+      <c r="K326" t="n">
+        <v>10</v>
+      </c>
+      <c r="L326" t="n">
+        <v>10</v>
+      </c>
+      <c r="M326" t="inlineStr">
+        <is>
+          <t>x_0</t>
+        </is>
+      </c>
+      <c r="N326" t="inlineStr">
+        <is>
+          <t>x_1</t>
+        </is>
+      </c>
+      <c r="O326" t="inlineStr">
+        <is>
+          <t>x_2</t>
+        </is>
+      </c>
+      <c r="P326" t="inlineStr">
+        <is>
+          <t>x_4</t>
+        </is>
+      </c>
+      <c r="Q326" t="inlineStr">
+        <is>
+          <t>x_6</t>
+        </is>
+      </c>
+      <c r="R326" t="inlineStr">
+        <is>
+          <t>y_r_142</t>
+        </is>
+      </c>
+      <c r="S326" t="inlineStr">
+        <is>
+          <t>y_r_145</t>
+        </is>
+      </c>
+      <c r="T326" t="inlineStr">
+        <is>
+          <t>y_r_147</t>
+        </is>
+      </c>
+      <c r="U326" t="inlineStr">
+        <is>
+          <t>y_r_24</t>
+        </is>
+      </c>
+      <c r="V326" t="inlineStr">
+        <is>
+          <t>y_r_27</t>
+        </is>
+      </c>
+      <c r="W326" t="inlineStr">
+        <is>
+          <t>y_r_31</t>
+        </is>
+      </c>
+      <c r="X326" t="inlineStr">
+        <is>
+          <t>y_r_35</t>
+        </is>
+      </c>
+      <c r="Y326" t="inlineStr">
+        <is>
+          <t>y_r_74</t>
+        </is>
+      </c>
+      <c r="Z326" t="inlineStr">
+        <is>
+          <t>y_r_85</t>
+        </is>
+      </c>
+      <c r="AA326" t="inlineStr">
+        <is>
+          <t>y_r_99</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>150</v>
+      </c>
+      <c r="B327" t="n">
+        <v>5</v>
+      </c>
+      <c r="C327" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>ER</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>test_files/SA1/ER/150/2.txt</t>
+        </is>
+      </c>
+      <c r="F327" t="n">
+        <v>8</v>
+      </c>
+      <c r="G327" t="n">
+        <v>10</v>
+      </c>
+      <c r="H327" t="n">
+        <v>10</v>
+      </c>
+      <c r="I327" t="n">
+        <v>10</v>
+      </c>
+      <c r="J327" t="n">
+        <v>10</v>
+      </c>
+      <c r="K327" t="n">
+        <v>10</v>
+      </c>
+      <c r="L327" t="n">
+        <v>10</v>
+      </c>
+      <c r="M327" t="inlineStr">
+        <is>
+          <t>x_0</t>
+        </is>
+      </c>
+      <c r="N327" t="inlineStr">
+        <is>
+          <t>x_1</t>
+        </is>
+      </c>
+      <c r="O327" t="inlineStr">
+        <is>
+          <t>x_2</t>
+        </is>
+      </c>
+      <c r="P327" t="inlineStr">
+        <is>
+          <t>x_4</t>
+        </is>
+      </c>
+      <c r="Q327" t="inlineStr">
+        <is>
+          <t>x_6</t>
+        </is>
+      </c>
+      <c r="R327" t="inlineStr">
+        <is>
+          <t>y_r_142</t>
+        </is>
+      </c>
+      <c r="S327" t="inlineStr">
+        <is>
+          <t>y_r_145</t>
+        </is>
+      </c>
+      <c r="T327" t="inlineStr">
+        <is>
+          <t>y_r_147</t>
+        </is>
+      </c>
+      <c r="U327" t="inlineStr">
+        <is>
+          <t>y_r_24</t>
+        </is>
+      </c>
+      <c r="V327" t="inlineStr">
+        <is>
+          <t>y_r_27</t>
+        </is>
+      </c>
+      <c r="W327" t="inlineStr">
+        <is>
+          <t>y_r_31</t>
+        </is>
+      </c>
+      <c r="X327" t="inlineStr">
+        <is>
+          <t>y_r_35</t>
+        </is>
+      </c>
+      <c r="Y327" t="inlineStr">
+        <is>
+          <t>y_r_74</t>
+        </is>
+      </c>
+      <c r="Z327" t="inlineStr">
+        <is>
+          <t>y_r_85</t>
+        </is>
+      </c>
+      <c r="AA327" t="inlineStr">
+        <is>
+          <t>y_r_99</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>150</v>
+      </c>
+      <c r="B328" t="n">
+        <v>5</v>
+      </c>
+      <c r="C328" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>ER</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>test_files/SA1/ER/150/2.txt</t>
+        </is>
+      </c>
+      <c r="F328" t="n">
+        <v>8</v>
+      </c>
+      <c r="G328" t="n">
+        <v>10</v>
+      </c>
+      <c r="H328" t="n">
+        <v>10</v>
+      </c>
+      <c r="I328" t="n">
+        <v>10</v>
+      </c>
+      <c r="J328" t="n">
+        <v>10</v>
+      </c>
+      <c r="K328" t="n">
+        <v>10</v>
+      </c>
+      <c r="L328" t="n">
+        <v>10</v>
+      </c>
+      <c r="M328" t="inlineStr">
+        <is>
+          <t>x_0</t>
+        </is>
+      </c>
+      <c r="N328" t="inlineStr">
+        <is>
+          <t>x_1</t>
+        </is>
+      </c>
+      <c r="O328" t="inlineStr">
+        <is>
+          <t>x_2</t>
+        </is>
+      </c>
+      <c r="P328" t="inlineStr">
+        <is>
+          <t>x_4</t>
+        </is>
+      </c>
+      <c r="Q328" t="inlineStr">
+        <is>
+          <t>x_6</t>
+        </is>
+      </c>
+      <c r="R328" t="inlineStr">
+        <is>
+          <t>y_r_142</t>
+        </is>
+      </c>
+      <c r="S328" t="inlineStr">
+        <is>
+          <t>y_r_145</t>
+        </is>
+      </c>
+      <c r="T328" t="inlineStr">
+        <is>
+          <t>y_r_147</t>
+        </is>
+      </c>
+      <c r="U328" t="inlineStr">
+        <is>
+          <t>y_r_24</t>
+        </is>
+      </c>
+      <c r="V328" t="inlineStr">
+        <is>
+          <t>y_r_27</t>
+        </is>
+      </c>
+      <c r="W328" t="inlineStr">
+        <is>
+          <t>y_r_31</t>
+        </is>
+      </c>
+      <c r="X328" t="inlineStr">
+        <is>
+          <t>y_r_35</t>
+        </is>
+      </c>
+      <c r="Y328" t="inlineStr">
+        <is>
+          <t>y_r_74</t>
+        </is>
+      </c>
+      <c r="Z328" t="inlineStr">
+        <is>
+          <t>y_r_85</t>
+        </is>
+      </c>
+      <c r="AA328" t="inlineStr">
         <is>
           <t>y_r_99</t>
         </is>
@@ -38053,7 +38521,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U324"/>
+  <dimension ref="A1:U328"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A296" ySplit="1"/>
@@ -51723,6 +52191,174 @@
       </c>
       <c r="L324" t="n">
         <v>0.03945920000000003</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>150</v>
+      </c>
+      <c r="B325" t="n">
+        <v>5</v>
+      </c>
+      <c r="C325" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>ER</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>test_files/SA1/ER/150/2.txt</t>
+        </is>
+      </c>
+      <c r="F325" t="n">
+        <v>0.0005870999999997295</v>
+      </c>
+      <c r="G325" t="n">
+        <v>7.789999999996411e-05</v>
+      </c>
+      <c r="H325" t="n">
+        <v>0.001861700000000077</v>
+      </c>
+      <c r="I325" t="n">
+        <v>0.06266380000000016</v>
+      </c>
+      <c r="J325" t="n">
+        <v>0.0002444000000001445</v>
+      </c>
+      <c r="K325" t="n">
+        <v>0.0002099000000002071</v>
+      </c>
+      <c r="L325" t="n">
+        <v>0.0249132000000003</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>150</v>
+      </c>
+      <c r="B326" t="n">
+        <v>5</v>
+      </c>
+      <c r="C326" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>ER</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>test_files/SA1/ER/150/2.txt</t>
+        </is>
+      </c>
+      <c r="F326" t="n">
+        <v>0.0005802999999999781</v>
+      </c>
+      <c r="G326" t="n">
+        <v>6.189999999994811e-05</v>
+      </c>
+      <c r="H326" t="n">
+        <v>0.001874500000000001</v>
+      </c>
+      <c r="I326" t="n">
+        <v>0.03176889999999999</v>
+      </c>
+      <c r="J326" t="n">
+        <v>0.0002473000000000614</v>
+      </c>
+      <c r="K326" t="n">
+        <v>0.0002109999999999612</v>
+      </c>
+      <c r="L326" t="n">
+        <v>0.03271420000000003</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>150</v>
+      </c>
+      <c r="B327" t="n">
+        <v>5</v>
+      </c>
+      <c r="C327" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>ER</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>test_files/SA1/ER/150/2.txt</t>
+        </is>
+      </c>
+      <c r="F327" t="n">
+        <v>0.0004842000000000457</v>
+      </c>
+      <c r="G327" t="n">
+        <v>3.629999999998912e-05</v>
+      </c>
+      <c r="H327" t="n">
+        <v>0.002175200000000044</v>
+      </c>
+      <c r="I327" t="n">
+        <v>0.04865770000000003</v>
+      </c>
+      <c r="J327" t="n">
+        <v>0.0003307000000001281</v>
+      </c>
+      <c r="K327" t="n">
+        <v>0.000265600000000088</v>
+      </c>
+      <c r="L327" t="n">
+        <v>0.02512350000000008</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>150</v>
+      </c>
+      <c r="B328" t="n">
+        <v>5</v>
+      </c>
+      <c r="C328" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>ER</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>test_files/SA1/ER/150/2.txt</t>
+        </is>
+      </c>
+      <c r="F328" t="n">
+        <v>0.002372400000000052</v>
+      </c>
+      <c r="G328" t="n">
+        <v>0.000322399999999945</v>
+      </c>
+      <c r="H328" t="n">
+        <v>0.01024340000000001</v>
+      </c>
+      <c r="I328" t="n">
+        <v>0.03325690000000003</v>
+      </c>
+      <c r="J328" t="n">
+        <v>35.283277</v>
+      </c>
+      <c r="K328" t="n">
+        <v>0.0007846000000029107</v>
+      </c>
+      <c r="L328" t="n">
+        <v>41.3841067</v>
       </c>
     </row>
   </sheetData>

</xml_diff>